<commit_message>
Edit ms. Add .xlsx version of Table 1.
</commit_message>
<xml_diff>
--- a/output/summary_table.xlsx
+++ b/output/summary_table.xlsx
@@ -1001,21 +1001,9 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1027,15 +1015,27 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1360,8 +1360,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,34 +1375,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1407,1255 +1410,1255 @@
       <c r="A2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>53</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>0.59599999999999997</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>-1.07</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="1">
         <v>-15.7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="1">
         <v>-14.8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>83</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>0.46</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>-2.41</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="1">
         <v>-20.100000000000001</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="1">
         <v>-18.100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>61</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>0.55600000000000005</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>-0.79900000000000004</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="1">
         <v>-17.100000000000001</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="1">
         <v>-16.399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>77</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="3">
         <v>0.56599999999999995</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="3">
         <v>-2.61</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="3">
         <v>-20.9</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="3">
         <v>-18.7</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>101</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.35899999999999999</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>-1.33</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="1">
         <v>-7.76</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <v>-6.52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>106</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>0.372</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>-2.13</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="1">
         <v>-9.3800000000000008</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="1">
         <v>-7.4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>95</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>-1.43</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="1">
         <v>-7.8</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="1">
         <v>-6.45</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="3">
         <v>108</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="3">
         <v>0.36899999999999999</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="3">
         <v>-0.64900000000000002</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="3">
         <v>-7.8</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="3">
         <v>-7.2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <v>61</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>0.46700000000000003</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>-1.54</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="1">
         <v>-4.68</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <v>-3.19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>30</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>0.39800000000000002</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>-1.17</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="1">
         <v>-4.66</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="1">
         <v>-3.53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <v>69</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>0.33400000000000002</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>-0.496</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="1">
         <v>-4.62</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="1">
         <v>-4.1399999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="3">
         <v>44</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="3">
         <v>0.34100000000000003</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="3">
         <v>-1.67</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="3">
         <v>-5</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="3">
         <v>-3.39</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>40</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <v>0.56899999999999995</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="1">
         <v>-0.59199999999999997</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="1">
         <v>-3.61</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="2">
         <v>9.1399999999999995E-2</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="1">
         <v>-3.03</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <v>29</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <v>0.67700000000000005</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="1">
         <v>-0.221</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="2">
         <v>8.72E-2</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="1">
         <v>-3.63</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="2">
         <v>0.13200000000000001</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="1">
         <v>-3.42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <v>64</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="1">
         <v>0.33700000000000002</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="1">
         <v>-1.2</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="1">
         <v>-3.97</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="1">
         <v>-2.8</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="3">
         <v>17</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="3">
         <v>0.65800000000000003</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="3">
         <v>-0.755</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="4">
         <v>0.13100000000000001</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="3">
         <v>-3.55</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="4">
         <v>0.218</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="3">
         <v>-2.82</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="7">
         <v>39</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="7">
         <v>0.57599999999999996</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="7">
         <v>-0.81499999999999995</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="8">
         <v>0.14199999999999999</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="7">
         <v>-3.44</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="8">
         <v>0.223</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="7">
         <v>-2.65</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>4</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="1">
         <v>0.68600000000000005</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="1">
         <v>-0.84799999999999998</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="2">
         <v>0.68600000000000005</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="1">
         <v>-3.41</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="2">
         <v>0.68600000000000005</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="1">
         <v>-2.58</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <v>7</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="1">
         <v>0.62</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="1">
         <v>-1.31</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <v>0.53500000000000003</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="1">
         <v>-3.58</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="2">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="1">
         <v>-2.2999999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="3">
         <v>43</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="3">
         <v>0.39900000000000002</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="3">
         <v>-0.97899999999999998</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="3">
         <v>-3.42</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="4">
         <v>9.9900000000000003E-2</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="3">
         <v>-2.4700000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="1">
         <v>68</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="1">
         <v>0.24299999999999999</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="1">
         <v>-0.53900000000000003</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="1">
         <v>-16</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="1">
         <v>-15.6</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="1">
         <v>5</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="1">
         <v>0.69</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="1">
         <v>-2.83</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>0.69</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="1">
         <v>-14.9</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="2">
         <v>0.69</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="1">
         <v>-12.4</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="3">
         <v>8</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="3">
         <v>0.64500000000000002</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="3">
         <v>-0.318</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="3">
         <v>-11.7</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="3">
         <v>-11.4</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="1">
         <v>81</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="1">
         <v>0.54400000000000004</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="1">
         <v>-0.52200000000000002</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="1">
         <v>-6.54</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="1">
         <v>-6.05</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="1">
         <v>50</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="1">
         <v>0.53700000000000003</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="1">
         <v>-1.1200000000000001</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="1">
         <v>-6.87</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="1">
         <v>-5.81</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="1">
         <v>44</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="1">
         <v>-2.4</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="1">
         <v>-5.64</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="1">
         <v>-3.31</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="1">
         <v>36</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="1">
         <v>0.52</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="1">
         <v>-0.23499999999999999</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="1">
         <v>-6.01</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="1">
         <v>-5.79</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="1">
         <v>14</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="1">
         <v>0.35199999999999998</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="1">
         <v>-1.77</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="1">
         <v>-6.31</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="1">
         <v>-4.62</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="3">
         <v>9</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="3">
         <v>0.73</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="3">
         <v>-0.68799999999999994</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="3">
         <v>-7.69</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="4">
         <v>9.3899999999999997E-2</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="3">
         <v>-7.06</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="12"/>
+      <c r="B31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="1">
         <v>186</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="1">
         <v>0.45900000000000002</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="1">
         <v>-0.56299999999999994</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="1">
         <v>-5.1100000000000003</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="1">
         <v>-4.57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="1">
         <v>61</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="1">
         <v>0.54200000000000004</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="1">
         <v>-0.47199999999999998</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="1">
         <v>-5.4</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="1">
         <v>-4.95</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="1">
         <v>187</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="1">
         <v>0.60899999999999999</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="1">
         <v>-0.624</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="1">
         <v>-5.18</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="1">
         <v>-4.58</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>52</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="1">
         <v>0.628</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="1">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="1">
         <v>-5.2</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="1">
         <v>-4.13</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="1">
         <v>28</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="1">
         <v>-0.94899999999999995</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="1">
         <v>-5</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="1">
         <v>-4.09</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7" t="s">
+      <c r="A36" s="12"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="3">
         <v>8</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="3">
         <v>0.72099999999999997</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="3">
         <v>-0.40100000000000002</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="4">
         <v>0.38200000000000001</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="3">
         <v>-4.91</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="4">
         <v>0.38200000000000001</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="3">
         <v>-4.53</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="1">
         <v>11</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="1">
         <v>0.748</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="1">
         <v>-0.25800000000000001</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="2">
         <v>0.217</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="1">
         <v>-4.79</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="2">
         <v>0.24299999999999999</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="1">
         <v>-4.54</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="1">
         <v>14</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="1">
         <v>0.748</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="1">
         <v>-2.4500000000000001E-2</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="1">
         <v>-4.68</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="1">
         <v>-4.66</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3" t="s">
+      <c r="A39" s="12"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>32</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="1">
         <v>0.63400000000000001</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="1">
         <v>-2.0299999999999998</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="2">
         <v>8.4500000000000006E-2</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="1">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="2">
         <v>0.17</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="1">
         <v>-2.62</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3" t="s">
+      <c r="A40" s="12"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="1">
         <v>7</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="1">
         <v>0.71</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="1">
         <v>-0.121</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="2">
         <v>0.45600000000000002</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="1">
         <v>-4.7699999999999996</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="2">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="1">
         <v>-4.66</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7" t="s">
+      <c r="A41" s="12"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="3">
         <v>8</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="3">
         <v>0.72099999999999997</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="3">
         <v>-0.36</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="4">
         <v>0.38200000000000001</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="3">
         <v>-4.71</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="4">
         <v>0.442</v>
       </c>
-      <c r="J41" s="7">
+      <c r="J41" s="3">
         <v>-4.37</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="12"/>
+      <c r="B42" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="1">
         <v>9</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="1">
         <v>0.73</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="1">
         <v>-6.4500000000000002E-2</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="2">
         <v>0.34</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="1">
         <v>-4.4800000000000004</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="2">
         <v>0.34</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="1">
         <v>-4.42</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3" t="s">
+      <c r="A43" s="12"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="1">
         <v>18</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="1">
         <v>-1.8</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="2">
         <v>0.111</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="1">
         <v>-4.5</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="2">
         <v>0.252</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="1">
         <v>-2.75</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="3" t="s">
+      <c r="A44" s="12"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="1">
         <v>4</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="1">
         <v>0.68600000000000005</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="1">
         <v>-2.1</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="2">
         <v>0.68600000000000005</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="1">
         <v>-4.51</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="2">
         <v>0.68600000000000005</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="1">
         <v>-2.4700000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7" t="s">
+      <c r="A45" s="13"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="3">
         <v>3</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="3">
         <v>0.4</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="3">
         <v>-3.37</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="4">
         <v>0.4</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="3">
         <v>-4.51</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="4">
         <v>0.50700000000000001</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="3">
         <v>-1.18</v>
       </c>
     </row>

</xml_diff>